<commit_message>
add true_clothes table for test
</commit_message>
<xml_diff>
--- a/Dataset/Clothes_table.xlsx
+++ b/Dataset/Clothes_table.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="504" windowWidth="20604" windowHeight="9468"/>
+    <workbookView xWindow="288" yWindow="24" windowWidth="20868" windowHeight="10080"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset_clothes" sheetId="1" r:id="rId1"/>
@@ -14,9 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="126">
-  <si>
-    <t>id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="125">
+  <si>
+    <t>id_clothes</t>
   </si>
   <si>
     <t>category</t>
@@ -286,7 +286,7 @@
     <t>gilet_5</t>
   </si>
   <si>
-    <t>Reste très simple et ducoup va avec tout. Petit gilet basique à avoir dans sa garde robe. Les petite rayures en transparence lui donnent un petit plus original.</t>
+    <t>Reste très simple et du coup va avec tout. Petit gilet basique à avoir dans sa garde robe. Les petite rayures en transparence lui donnent un petit plus original.</t>
   </si>
   <si>
     <t>gilet_6</t>
@@ -380,9 +380,6 @@
   </si>
   <si>
     <t>pantalon_7</t>
-  </si>
-  <si>
-    <t>jogging</t>
   </si>
   <si>
     <t xml:space="preserve">Parfaitement adapté pour des journées chill à la maison, ou bien pour aller se promener en demi saison ou hiver </t>
@@ -402,7 +399,7 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -413,7 +410,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -425,17 +422,17 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1A1A1A"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,6 +443,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -461,20 +464,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,56 +489,114 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -546,131 +608,160 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -691,9 +782,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
-    <col min="2" max="2" width="8.77734375" customWidth="1"/>
-    <col min="3" max="3" width="194.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="194.77734375" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="12.6640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" customHeight="1">
@@ -706,25 +798,25 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
@@ -733,28 +825,28 @@
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
@@ -763,28 +855,28 @@
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
     </row>
     <row r="4" spans="1:22" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
@@ -793,28 +885,28 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
@@ -823,28 +915,28 @@
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
     </row>
     <row r="6" spans="1:22" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
@@ -853,28 +945,28 @@
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
@@ -883,28 +975,28 @@
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
@@ -913,28 +1005,28 @@
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
     </row>
     <row r="9" spans="1:22" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -943,28 +1035,28 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
     </row>
     <row r="10" spans="1:22" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
@@ -973,28 +1065,28 @@
       <c r="B10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:22" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
@@ -1003,28 +1095,28 @@
       <c r="B11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
@@ -1033,28 +1125,28 @@
       <c r="B12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
@@ -1063,28 +1155,28 @@
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-      <c r="S13" s="2"/>
-      <c r="T13" s="2"/>
-      <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
@@ -1093,28 +1185,28 @@
       <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="2"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="2"/>
-      <c r="U14" s="2"/>
-      <c r="V14" s="2"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
@@ -1123,28 +1215,28 @@
       <c r="B15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="2"/>
-      <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
@@ -1153,28 +1245,28 @@
       <c r="B16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
@@ -1183,28 +1275,28 @@
       <c r="B17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
@@ -1213,28 +1305,28 @@
       <c r="B18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="2"/>
-      <c r="V18" s="2"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
@@ -1243,28 +1335,28 @@
       <c r="B19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="2"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="2"/>
-      <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
@@ -1273,28 +1365,28 @@
       <c r="B20" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-      <c r="O20" s="2"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="2"/>
-      <c r="U20" s="2"/>
-      <c r="V20" s="2"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
@@ -1303,48 +1395,48 @@
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
-      <c r="O21" s="2"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="2"/>
-      <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-    </row>
-    <row r="22" spans="1:22">
-      <c r="A22" s="3" t="s">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="1:22" ht="14.4">
+      <c r="A22" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1355,7 +1447,7 @@
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1366,384 +1458,384 @@
       <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C25" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:22" ht="13.8">
+      <c r="A26" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:22" ht="13.8">
+      <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:22" ht="13.8">
+      <c r="A28" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
-      <c r="A29" s="3" t="s">
+    <row r="29" spans="1:22" ht="13.8">
+      <c r="A29" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
-      <c r="A30" s="3" t="s">
+    <row r="30" spans="1:22" ht="13.8">
+      <c r="A30" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
-      <c r="A31" s="3" t="s">
+    <row r="31" spans="1:22" ht="13.8">
+      <c r="A31" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="5" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:22" ht="13.8">
+      <c r="A32" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="3" t="s">
+    <row r="33" spans="1:3" ht="13.8">
+      <c r="A33" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="5" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="5" t="s">
         <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="5" t="s">
         <v>81</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="3" t="s">
+    <row r="38" spans="1:3" ht="13.8">
+      <c r="A38" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="3" t="s">
+    <row r="39" spans="1:3" ht="13.8">
+      <c r="A39" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="3" t="s">
+    <row r="40" spans="1:3" ht="13.8">
+      <c r="A40" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="C40" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:3" ht="13.8">
+      <c r="A41" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="3" t="s">
+    <row r="42" spans="1:3" ht="13.8">
+      <c r="A42" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="3" t="s">
+    <row r="43" spans="1:3" ht="13.8">
+      <c r="A43" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="3" t="s">
+    <row r="44" spans="1:3" ht="13.8">
+      <c r="A44" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C44" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:3" ht="13.8">
+      <c r="A45" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="3" t="s">
+    <row r="46" spans="1:3" ht="13.8">
+      <c r="A46" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="5" t="s">
+    <row r="47" spans="1:3" ht="13.8">
+      <c r="A47" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="3" t="s">
+    <row r="48" spans="1:3" ht="13.8">
+      <c r="A48" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:3" ht="13.8">
+      <c r="A49" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:3" ht="13.8">
+      <c r="A50" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="3" t="s">
+    <row r="51" spans="1:3" ht="13.8">
+      <c r="A51" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:3" ht="13.8">
+      <c r="A52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="3" t="s">
+    <row r="53" spans="1:3" ht="13.8">
+      <c r="A53" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="3" t="s">
+    <row r="54" spans="1:3" ht="13.8">
+      <c r="A54" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="3" t="s">
+    <row r="55" spans="1:3" ht="13.8">
+      <c r="A55" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C55" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="3" t="s">
+    <row r="56" spans="1:3" ht="13.8">
+      <c r="A56" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="3" t="s">
+    </row>
+    <row r="57" spans="1:3" ht="13.8">
+      <c r="A57" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="3" t="s">
+      <c r="B57" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C19:Q19"/>
     <mergeCell ref="C20:K20"/>
     <mergeCell ref="C21:K21"/>
+    <mergeCell ref="C14:Q14"/>
+    <mergeCell ref="C15:M15"/>
+    <mergeCell ref="C16:L16"/>
+    <mergeCell ref="C17:P17"/>
+    <mergeCell ref="C18:T18"/>
+    <mergeCell ref="C19:Q19"/>
+    <mergeCell ref="C8:N8"/>
     <mergeCell ref="C9:Q9"/>
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="C11:J11"/>
     <mergeCell ref="C12:I12"/>
     <mergeCell ref="C13:L13"/>
-    <mergeCell ref="C14:Q14"/>
-    <mergeCell ref="C15:M15"/>
-    <mergeCell ref="C7:N7"/>
-    <mergeCell ref="C8:N8"/>
-    <mergeCell ref="C16:L16"/>
-    <mergeCell ref="C17:P17"/>
-    <mergeCell ref="C18:T18"/>
     <mergeCell ref="C2:H2"/>
     <mergeCell ref="C3:G3"/>
     <mergeCell ref="C4:J4"/>
     <mergeCell ref="C5:H5"/>
     <mergeCell ref="C6:O6"/>
+    <mergeCell ref="C7:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>